<commit_message>
Update to the whole main.py
</commit_message>
<xml_diff>
--- a/output/emails.xlsx
+++ b/output/emails.xlsx
@@ -701,7 +701,11 @@
           <t>15708517-4</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -717,7 +721,11 @@
           <t>16430202-4</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -733,7 +741,11 @@
           <t>23451436-9</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -749,7 +761,11 @@
           <t>27731474-6</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -765,7 +781,11 @@
           <t>6907565-7</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -781,7 +801,11 @@
           <t>19694694-2</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -797,7 +821,11 @@
           <t>12286228-3</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -813,7 +841,11 @@
           <t>7599323-4</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -829,7 +861,11 @@
           <t>20107416-9</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -845,7 +881,11 @@
           <t>13450130-8</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -2241,9 +2281,19 @@
           <t>47128577-3</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2251,9 +2301,19 @@
           <t>15224127-5</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2261,9 +2321,19 @@
           <t>22122985-1</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2271,9 +2341,19 @@
           <t>48825804-4</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2281,9 +2361,19 @@
           <t>7791076-K</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr"/>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2291,9 +2381,19 @@
           <t>9664417-5</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr"/>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2301,9 +2401,19 @@
           <t>37732660-1</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr"/>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2311,9 +2421,19 @@
           <t>38062614-4</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2321,9 +2441,19 @@
           <t>34084266-9</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr"/>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2331,9 +2461,19 @@
           <t>43684610-K</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr"/>
-      <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr"/>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2341,9 +2481,19 @@
           <t>45565314-2</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr"/>
-      <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr"/>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4091,7 +4241,11 @@
           <t>16320355-3</t>
         </is>
       </c>
-      <c r="B191" t="inlineStr"/>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C191" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -4107,7 +4261,11 @@
           <t>43293568-K</t>
         </is>
       </c>
-      <c r="B192" t="inlineStr"/>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C192" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4123,7 +4281,11 @@
           <t>17681862-K</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr"/>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C193" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4139,7 +4301,11 @@
           <t>50322835-1</t>
         </is>
       </c>
-      <c r="B194" t="inlineStr"/>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C194" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4155,7 +4321,11 @@
           <t>18630836-0</t>
         </is>
       </c>
-      <c r="B195" t="inlineStr"/>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C195" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4171,7 +4341,11 @@
           <t>5390199-9</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr"/>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C196" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4187,7 +4361,11 @@
           <t>25005157-3</t>
         </is>
       </c>
-      <c r="B197" t="inlineStr"/>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C197" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -4203,7 +4381,11 @@
           <t>23571025-0</t>
         </is>
       </c>
-      <c r="B198" t="inlineStr"/>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C198" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4219,7 +4401,11 @@
           <t>20777151-1</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr"/>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C199" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4235,7 +4421,11 @@
           <t>20583506-7</t>
         </is>
       </c>
-      <c r="B200" t="inlineStr"/>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C200" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -4251,7 +4441,11 @@
           <t>42619550-K</t>
         </is>
       </c>
-      <c r="B201" t="inlineStr"/>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C201" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4267,7 +4461,11 @@
           <t>29260415-7</t>
         </is>
       </c>
-      <c r="B202" t="inlineStr"/>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C202" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -4283,7 +4481,11 @@
           <t>26484586-6</t>
         </is>
       </c>
-      <c r="B203" t="inlineStr"/>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C203" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -4299,7 +4501,11 @@
           <t>8383850-7</t>
         </is>
       </c>
-      <c r="B204" t="inlineStr"/>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C204" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4315,7 +4521,11 @@
           <t>18579699-K</t>
         </is>
       </c>
-      <c r="B205" t="inlineStr"/>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C205" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -4331,7 +4541,11 @@
           <t>48327335-5</t>
         </is>
       </c>
-      <c r="B206" t="inlineStr"/>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C206" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -11967,9 +12181,19 @@
           <t>43451887-3</t>
         </is>
       </c>
-      <c r="B588" t="inlineStr"/>
-      <c r="C588" t="inlineStr"/>
-      <c r="D588" t="inlineStr"/>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D588" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="589">
       <c r="A589" t="inlineStr">
@@ -11977,9 +12201,19 @@
           <t>32571740-8</t>
         </is>
       </c>
-      <c r="B589" t="inlineStr"/>
-      <c r="C589" t="inlineStr"/>
-      <c r="D589" t="inlineStr"/>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D589" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="590">
       <c r="A590" t="inlineStr">
@@ -11987,9 +12221,19 @@
           <t>25667290-1</t>
         </is>
       </c>
-      <c r="B590" t="inlineStr"/>
-      <c r="C590" t="inlineStr"/>
-      <c r="D590" t="inlineStr"/>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D590" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="591">
       <c r="A591" t="inlineStr">
@@ -11997,9 +12241,19 @@
           <t>35815242-2</t>
         </is>
       </c>
-      <c r="B591" t="inlineStr"/>
-      <c r="C591" t="inlineStr"/>
-      <c r="D591" t="inlineStr"/>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D591" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="592">
       <c r="A592" t="inlineStr">
@@ -12067,7 +12321,11 @@
           <t>24195304-1</t>
         </is>
       </c>
-      <c r="B595" t="inlineStr"/>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C595" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -12083,7 +12341,11 @@
           <t>43177273-6</t>
         </is>
       </c>
-      <c r="B596" t="inlineStr"/>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C596" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -12099,7 +12361,11 @@
           <t>48121035-6</t>
         </is>
       </c>
-      <c r="B597" t="inlineStr"/>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C597" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -12115,7 +12381,11 @@
           <t>32761397-9</t>
         </is>
       </c>
-      <c r="B598" t="inlineStr"/>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C598" t="inlineStr">
         <is>
           <t>VALIDO</t>
@@ -12131,7 +12401,11 @@
           <t>43471829-5</t>
         </is>
       </c>
-      <c r="B599" t="inlineStr"/>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C599" t="inlineStr">
         <is>
           <t>INVALIDO</t>
@@ -12147,7 +12421,11 @@
           <t>42169978-K</t>
         </is>
       </c>
-      <c r="B600" t="inlineStr"/>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C600" t="inlineStr">
         <is>
           <t>INVALIDO</t>

</xml_diff>